<commit_message>
Added Remap for Fischl and FischlHighness
- For FischlHighness --> Fischl, had to sacrifice the lustre on metal
parts of Fischl's head for better shadow on her hair. Fischl does not
have any metal map texture while FischlHighness does. So the crown
on Fischl may seem like transparent

- Fix bug with the "GIMISplitFixer" to fix sections with their
registers editted
</commit_message>
<xml_diff>
--- a/Data/RemapDrafts/JeanRemapDraft.xlsx
+++ b/Data/RemapDrafts/JeanRemapDraft.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Computer\Games\Genshin\Repos\Repos\Fix-Raiden-Boss-Fork\Data\RemapDrafts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Computer\Games\Genshin\Repos\Repos\Fix-Raiden-Boss\Data\RemapDrafts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530D6996-4A60-40C2-B622-5AA585D29F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264846FC-4AC1-44C0-B04A-744BEA7E3CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="13900" activeTab="3" xr2:uid="{B08DB923-5719-4BE6-B084-9B7B07E846C8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Jean to JeanSeaBreeze" sheetId="1" r:id="rId1"/>
-    <sheet name="JeanCN to JeanSeaBreeze" sheetId="2" r:id="rId2"/>
-    <sheet name="JeanSeaBreeze to JeanCN" sheetId="3" r:id="rId3"/>
-    <sheet name="JeanSeaBreeze to Jean" sheetId="5" r:id="rId4"/>
+    <sheet name="V4.0 Jean to JeanSeaBreeze" sheetId="1" r:id="rId1"/>
+    <sheet name="V4.0 JeanCN to JeanSeaBreeze" sheetId="2" r:id="rId2"/>
+    <sheet name="V4.0 JeanSeaBreeze to JeanCN" sheetId="3" r:id="rId3"/>
+    <sheet name="V4.0 JeanSeaBreeze to Jean" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Jean to JeanSeaBreeze'!$A$1:$D$106</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'JeanCN to JeanSeaBreeze'!$A$1:$D$106</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'JeanSeaBreeze to Jean'!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'JeanSeaBreeze to JeanCN'!$A$1:$D$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'V4.0 Jean to JeanSeaBreeze'!$A$1:$D$106</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'V4.0 JeanCN to JeanSeaBreeze'!$A$1:$D$106</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'V4.0 JeanSeaBreeze to Jean'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'V4.0 JeanSeaBreeze to JeanCN'!$A$1:$D$86</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
   <si>
     <t>Uncertainty</t>
   </si>
@@ -189,6 +189,24 @@
   </si>
   <si>
     <t>JeanSea's right toes</t>
+  </si>
+  <si>
+    <t>JeanSea's right ankle</t>
+  </si>
+  <si>
+    <t>JeanSea's right bottom leg</t>
+  </si>
+  <si>
+    <t>JeanSea's left ankle</t>
+  </si>
+  <si>
+    <t>JeanSea's left bottom leg</t>
+  </si>
+  <si>
+    <t>JeanSea's right upper leg</t>
+  </si>
+  <si>
+    <t>JeanSea's left upper leg</t>
   </si>
 </sst>
 </file>
@@ -593,7 +611,7 @@
   <dimension ref="A1:D106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" sqref="A1:A106"/>
     </sheetView>
@@ -1604,7 +1622,7 @@
   <dimension ref="A1:D106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -3304,8 +3322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8AA5F56-F749-41C7-A993-BD2A5016016C}">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3577,7 +3595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>31</v>
       </c>
@@ -3585,7 +3603,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>32</v>
       </c>
@@ -3593,7 +3611,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>33</v>
       </c>
@@ -3601,7 +3619,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>34</v>
       </c>
@@ -3609,7 +3627,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>35</v>
       </c>
@@ -3617,7 +3635,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>36</v>
       </c>
@@ -3625,15 +3643,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39">
         <v>98</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>38</v>
       </c>
@@ -3641,7 +3662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>39</v>
       </c>
@@ -3649,7 +3670,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>40</v>
       </c>
@@ -3657,7 +3678,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>41</v>
       </c>
@@ -3665,7 +3686,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>42</v>
       </c>
@@ -3673,7 +3694,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>43</v>
       </c>
@@ -3681,7 +3702,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>44</v>
       </c>
@@ -3689,7 +3710,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>45</v>
       </c>
@@ -3697,7 +3718,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>46</v>
       </c>
@@ -3705,7 +3726,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>47</v>
       </c>
@@ -3713,7 +3734,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>48</v>
       </c>
@@ -3721,7 +3742,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>49</v>
       </c>
@@ -3729,7 +3750,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>50</v>
       </c>
@@ -3737,7 +3758,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>51</v>
       </c>
@@ -3745,7 +3766,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>52</v>
       </c>
@@ -3753,7 +3774,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>53</v>
       </c>
@@ -3761,15 +3782,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56">
         <v>99</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D56" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>55</v>
       </c>
@@ -3777,7 +3801,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>56</v>
       </c>
@@ -3785,15 +3809,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="B59">
         <v>97</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D59" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>58</v>
       </c>
@@ -3801,7 +3828,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>59</v>
       </c>
@@ -3809,15 +3836,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="B62">
         <v>102</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D62" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>61</v>
       </c>
@@ -3825,7 +3855,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>62</v>
       </c>
@@ -3833,7 +3863,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>63</v>
       </c>
@@ -3841,7 +3871,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>64</v>
       </c>
@@ -3849,7 +3879,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3857,7 +3887,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>66</v>
       </c>
@@ -3865,7 +3895,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3873,7 +3903,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3881,7 +3911,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>69</v>
       </c>
@@ -3889,7 +3919,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>70</v>
       </c>
@@ -3897,7 +3927,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>71</v>
       </c>
@@ -3905,7 +3935,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>72</v>
       </c>
@@ -3913,7 +3943,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>73</v>
       </c>
@@ -3921,7 +3951,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>74</v>
       </c>
@@ -3929,7 +3959,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>75</v>
       </c>
@@ -3937,7 +3967,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>76</v>
       </c>
@@ -3945,15 +3975,18 @@
         <v>63</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>77</v>
       </c>
       <c r="B79">
         <v>103</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D79" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>78</v>
       </c>
@@ -3961,7 +3994,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>79</v>
       </c>
@@ -3969,15 +4002,18 @@
         <v>48</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>80</v>
       </c>
       <c r="B82">
         <v>101</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D82" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>81</v>
       </c>
@@ -3985,7 +4021,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>82</v>
       </c>
@@ -3993,7 +4029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>83</v>
       </c>
@@ -4001,7 +4037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>84</v>
       </c>

</xml_diff>